<commit_message>
style: form process info created
</commit_message>
<xml_diff>
--- a/PropProAssistant/Test/WorksheetModels/LicitaNet/LN_03.xlsx
+++ b/PropProAssistant/Test/WorksheetModels/LicitaNet/LN_03.xlsx
@@ -15,12 +15,12 @@
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="15">
   <si>
     <t>LOTE</t>
   </si>
@@ -71,8 +71,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -101,11 +100,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="4" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,15 +417,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="70" customWidth="1" style="1"/>
+    <col min="3" max="3" width="70" style="1" customWidth="1"/>
     <col min="7" max="7" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -435,10 +434,10 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -447,11 +446,11 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2">
-      <c r="A2" s="0">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <v>3102298</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -460,21 +459,21 @@
       <c r="D2" s="2">
         <v>5</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="0">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="0">
+      <c r="B3">
         <v>3102299</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -483,21 +482,21 @@
       <c r="D3" s="2">
         <v>1400</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="0">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <v>3102300</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -506,21 +505,21 @@
       <c r="D4" s="2">
         <v>150</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="0" t="s">
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="0">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>3102301</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -529,21 +528,21 @@
       <c r="D5" s="2">
         <v>150</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="0" t="s">
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
         <v>7</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="0">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="0">
+      <c r="B6">
         <v>3102302</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -552,21 +551,21 @@
       <c r="D6" s="2">
         <v>12</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="0" t="s">
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
         <v>7</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="0">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="0">
+      <c r="B7">
         <v>3102303</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -575,21 +574,21 @@
       <c r="D7" s="2">
         <v>378</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="0" t="s">
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="0">
-        <v>7</v>
-      </c>
-      <c r="B8" s="0">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>3102304</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -598,21 +597,21 @@
       <c r="D8" s="2">
         <v>316</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="0" t="s">
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="0">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="0">
+      <c r="B9">
         <v>3102305</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -621,21 +620,21 @@
       <c r="D9" s="2">
         <v>250</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="0" t="s">
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="0">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="0">
+      <c r="B10">
         <v>3102306</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -644,21 +643,21 @@
       <c r="D10" s="2">
         <v>560</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="0" t="s">
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
         <v>7</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="0">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="0">
+      <c r="B11">
         <v>3102307</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -667,21 +666,21 @@
       <c r="D11" s="2">
         <v>520</v>
       </c>
-      <c r="E11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="0" t="s">
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
         <v>7</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="0">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="0">
+      <c r="B12">
         <v>3102308</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -690,21 +689,21 @@
       <c r="D12" s="2">
         <v>315</v>
       </c>
-      <c r="E12" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="0" t="s">
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
         <v>7</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="0">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="0">
+      <c r="B13">
         <v>3102309</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -713,21 +712,21 @@
       <c r="D13" s="2">
         <v>624</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="0" t="s">
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
         <v>7</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="0">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="0">
+      <c r="B14">
         <v>3102310</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -736,21 +735,21 @@
       <c r="D14" s="2">
         <v>3125</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="0" t="s">
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
         <v>7</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="0">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="0">
+      <c r="B15">
         <v>3102311</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -759,21 +758,21 @@
       <c r="D15" s="2">
         <v>1000</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="0" t="s">
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
         <v>7</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="0">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="0">
+      <c r="B16">
         <v>3102312</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -782,21 +781,21 @@
       <c r="D16" s="2">
         <v>524</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="0" t="s">
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
         <v>7</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="0">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="0">
+      <c r="B17">
         <v>3102313</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -805,21 +804,21 @@
       <c r="D17" s="2">
         <v>650</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="0" t="s">
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
         <v>7</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="0">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="0">
+      <c r="B18">
         <v>3102314</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -828,21 +827,21 @@
       <c r="D18" s="2">
         <v>610</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="0" t="s">
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
         <v>7</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="0">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="0">
+      <c r="B19">
         <v>3102315</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -851,21 +850,21 @@
       <c r="D19" s="2">
         <v>4400</v>
       </c>
-      <c r="E19" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="0" t="s">
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
         <v>7</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="0">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="0">
+      <c r="B20">
         <v>3102316</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -874,21 +873,21 @@
       <c r="D20" s="2">
         <v>2200</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="0" t="s">
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
         <v>7</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="0">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="0">
+      <c r="B21">
         <v>3102317</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -897,10 +896,10 @@
       <c r="D21" s="2">
         <v>42000</v>
       </c>
-      <c r="E21" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="0" t="s">
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" t="s">
         <v>7</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -910,6 +909,5 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>